<commit_message>
add excel file write function
</commit_message>
<xml_diff>
--- a/doc/template.xlsx
+++ b/doc/template.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msp\hrm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750B655D-E4F4-4F78-AABF-82BB621AD735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,18 +124,69 @@
     </r>
     <r>
       <rPr>
+        <rFont val="黑体"/>
+        <color theme="1"/>
         <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="黑体"/>
       </rPr>
       <t>1)如何在Excel中输入身份证号码,我们在Excel中输入身份证号码时,通常会遇到这样的问题,由于输入的身份证号码过长.</t>
     </r>
+  </si>
+  <si>
+    <t>李四</t>
+  </si>
+  <si>
+    <t>女</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>3年</t>
+  </si>
+  <si>
+    <t>3800</t>
+  </si>
+  <si>
+    <t>开发部</t>
+  </si>
+  <si>
+    <t>无</t>
+  </si>
+  <si>
+    <t>13866666666</t>
+  </si>
+  <si>
+    <t>蓝盾</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>高职</t>
+  </si>
+  <si>
+    <t>党员</t>
+  </si>
+  <si>
+    <t>7654321</t>
+  </si>
+  <si>
+    <t>54321</t>
+  </si>
+  <si>
+    <t>广西省南宁市江南区华夏街道180号</t>
+  </si>
+  <si>
+    <t>1、近日,全国两会受到了社会各界的广泛关注</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -151,7 +201,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -159,7 +209,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -174,7 +224,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="黑体"/>
@@ -345,52 +395,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -398,7 +448,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -411,154 +461,154 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 主题​​">
+  <themeElements>
+    <clrScheme name="Office">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="1F497D"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="EEECE1"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="4F81BD"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="C0504D"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="9BBB59"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="8064A2"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="4BACC6"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="F79646"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0000FF"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="800080"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office">
+      <majorFont>
+        <latin typeface="Cambria" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="宋体"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+        <font script="Armn" typeface="Arial"/>
+        <font script="Bugi" typeface="Leelawadee UI"/>
+        <font script="Bopo" typeface="Microsoft JhengHei"/>
+        <font script="Java" typeface="Javanese Text"/>
+        <font script="Lisu" typeface="Segoe UI"/>
+        <font script="Mymr" typeface="Myanmar Text"/>
+        <font script="Nkoo" typeface="Ebrima"/>
+        <font script="Olck" typeface="Nirmala UI"/>
+        <font script="Osma" typeface="Ebrima"/>
+        <font script="Phag" typeface="Phagspa"/>
+        <font script="Syrn" typeface="Estrangelo Edessa"/>
+        <font script="Syrj" typeface="Estrangelo Edessa"/>
+        <font script="Syre" typeface="Estrangelo Edessa"/>
+        <font script="Sora" typeface="Nirmala UI"/>
+        <font script="Tale" typeface="Microsoft Tai Le"/>
+        <font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <font script="Tfng" typeface="Ebrima"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="宋体"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+        <font script="Armn" typeface="Arial"/>
+        <font script="Bugi" typeface="Leelawadee UI"/>
+        <font script="Bopo" typeface="Microsoft JhengHei"/>
+        <font script="Java" typeface="Javanese Text"/>
+        <font script="Lisu" typeface="Segoe UI"/>
+        <font script="Mymr" typeface="Myanmar Text"/>
+        <font script="Nkoo" typeface="Ebrima"/>
+        <font script="Olck" typeface="Nirmala UI"/>
+        <font script="Osma" typeface="Ebrima"/>
+        <font script="Phag" typeface="Phagspa"/>
+        <font script="Syrn" typeface="Estrangelo Edessa"/>
+        <font script="Syrj" typeface="Estrangelo Edessa"/>
+        <font script="Syre" typeface="Estrangelo Edessa"/>
+        <font script="Sora" typeface="Nirmala UI"/>
+        <font script="Tale" typeface="Microsoft Tai Le"/>
+        <font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <font script="Tfng" typeface="Ebrima"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -608,8 +658,8 @@
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
@@ -631,8 +681,8 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
@@ -671,8 +721,8 @@
             <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -721,32 +771,32 @@
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="12.77734375"/>
+    <col customWidth="true" max="2" min="2" width="15.109375"/>
+    <col customWidth="true" max="3" min="3" width="11.21875"/>
+    <col customWidth="true" max="4" min="4" width="29.33203125"/>
+    <col customWidth="true" max="6" min="6" width="18.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="54.75" customHeight="1">
+    <row r="1" spans="1:6" ht="54.75" customHeight="true">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -756,121 +806,121 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1">
+    <row r="2" spans="1:6" ht="30" customHeight="true">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1">
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="true">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
-        <v>3600</v>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3">
-        <v>13899999999</v>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="true">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
-        <v>173</v>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2">
-        <v>70</v>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="true">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2">
-        <v>123456789</v>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2">
-        <v>1234567</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
+      <c r="F6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="true">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
+    <row r="8" spans="1:6" ht="30" customHeight="true">
       <c r="A8" s="8" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -878,7 +928,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1">
+    <row r="9" spans="1:6" ht="30" customHeight="true">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -886,7 +936,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
+    <row r="10" spans="1:6" ht="30" customHeight="true">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -894,7 +944,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" ht="369.75" customHeight="1">
+    <row r="11" spans="1:6" ht="369.75" customHeight="true">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -909,8 +959,8 @@
     <mergeCell ref="A8:F11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.9055118110236221" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.9055118110236221" right="0.7086614173228347" top="0.7480314960629921" bottom="0.7480314960629921" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup r:id="rId1" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 

</xml_diff>